<commit_message>
latest version 0.0.14 updated assignment algorithm
</commit_message>
<xml_diff>
--- a/exampleProblems/Canadine/Canadine.xlsx
+++ b/exampleProblems/Canadine/Canadine.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/vsmw51_durham_ac_uk/Documents/projects/programming/2022/python/python/rdkit37/projects/simpleNMR/exampleProblems/Canadine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{DDE66525-C75F-6D40-B1EC-C5D1BB045B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98890EB9-FD0D-4329-8D80-BB4A5B8C4F65}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{DDE66525-C75F-6D40-B1EC-C5D1BB045B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E01A9885-2980-40F8-9286-8648739DF7A1}"/>
   <bookViews>
-    <workbookView xWindow="1305" yWindow="795" windowWidth="14505" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="molecule" sheetId="9" r:id="rId1"/>
@@ -677,7 +677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -708,12 +708,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection sqref="A1:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4424,12 +4425,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4650,15 +4648,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9421959D-9476-4FEC-BDFE-1367083D3EBE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44668820-0664-4E62-A660-376AF03334EF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b60d6f15-5eb1-4c0b-bb71-d899d3bf026f"/>
+    <ds:schemaRef ds:uri="f6191221-55a2-427d-afce-6bfcc029a585"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4683,18 +4693,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44668820-0664-4E62-A660-376AF03334EF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9421959D-9476-4FEC-BDFE-1367083D3EBE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b60d6f15-5eb1-4c0b-bb71-d899d3bf026f"/>
-    <ds:schemaRef ds:uri="f6191221-55a2-427d-afce-6bfcc029a585"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>